<commit_message>
Mejora de plot y logos paquetes
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\kk\new_website_ECOINF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DC9E2F-B1CA-4E62-8B66-1D7E8109FC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCC0F2B-3728-4BFA-9120-EFA449386765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,31 +39,31 @@
     <t>type</t>
   </si>
   <si>
-    <t>creación</t>
-  </si>
-  <si>
     <t>Primera nota ecoinformática</t>
   </si>
   <si>
-    <t>publicaciones</t>
-  </si>
-  <si>
-    <t>seminario</t>
-  </si>
-  <si>
     <t>Primer Seminario Ecoinformático</t>
   </si>
   <si>
     <t>V Aniversario del grupo</t>
   </si>
   <si>
-    <t>curso</t>
-  </si>
-  <si>
     <t>Creación del grupo de Ecoinformática</t>
   </si>
   <si>
     <t xml:space="preserve">Primeras Jornadas Ecoinformáticas </t>
+  </si>
+  <si>
+    <t>Creación</t>
+  </si>
+  <si>
+    <t>Publicaciones</t>
+  </si>
+  <si>
+    <t>Seminarios</t>
+  </si>
+  <si>
+    <t>Cursos</t>
   </si>
 </sst>
 </file>
@@ -384,7 +384,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -414,10 +414,10 @@
         <v>2017</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -428,10 +428,10 @@
         <v>2017</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -442,10 +442,10 @@
         <v>2022</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -456,10 +456,10 @@
         <v>2022</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
@@ -470,10 +470,10 @@
         <v>2024</v>
       </c>
       <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion links seminarios y notas ecoinformaticas
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\kk\new_website_ECOINF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E750EF5-00F7-4E90-A2B1-78AA459C3D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9381E-3B3C-43D8-B635-F6B3B0466201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
   <si>
     <t>month</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Seminarios</t>
   </si>
   <si>
-    <t>Nota ecoinformática</t>
-  </si>
-  <si>
     <t>link</t>
   </si>
   <si>
@@ -100,6 +97,57 @@
   </si>
   <si>
     <t>https://ecoinf.quarto.pub/iecoinf/</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=VSUEi50tkAI</t>
+  </si>
+  <si>
+    <t>Notas ecoinformáticas</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=usB7reMJxLU</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=OKEtldANpHA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=niPkyIrEv-k</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=oAC7DVWAMRc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=0_73g05Wjgc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ybD4GM_OB3M</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=1ye4v3ugAfc</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=ZwKuy6E-GhE</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=nkEM6ny_E9U</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=C9Gyah5XES0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Fy5YNSe-btA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=CPimYLdDI5o</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=vzjqLjKOPPM</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=KLN2wMnivVA</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=txJfuPeodQw</t>
   </si>
 </sst>
 </file>
@@ -428,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -451,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -467,270 +515,483 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>2017</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B6">
         <v>2017</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>2018</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>2018</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>2019</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B12">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B13">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2020</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>2021</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B18">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B19">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B20">
         <v>2024</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B21">
+        <v>2022</v>
+      </c>
+      <c r="C21" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>2022</v>
+      </c>
+      <c r="C22" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>2022</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>2022</v>
+      </c>
+      <c r="C24" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>2022</v>
+      </c>
+      <c r="C25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>7</v>
+      </c>
+      <c r="B26">
+        <v>2022</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>2022</v>
+      </c>
+      <c r="C27" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>10</v>
+      </c>
+      <c r="B28">
+        <v>2022</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>11</v>
+      </c>
+      <c r="B29">
+        <v>2022</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>2023</v>
+      </c>
+      <c r="C30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>2023</v>
+      </c>
+      <c r="C31" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32">
+        <v>2023</v>
+      </c>
+      <c r="C32" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
         <v>2024</v>
       </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21" t="s">
-        <v>20</v>
+      <c r="C33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>2024</v>
+      </c>
+      <c r="C34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>2024</v>
+      </c>
+      <c r="C35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>2024</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{B5274820-F334-49F2-9C65-BC403D5350B7}"/>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{B5274820-F334-49F2-9C65-BC403D5350B7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
actualizacion datos y script
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\kk\new_website_ECOINF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8C9381E-3B3C-43D8-B635-F6B3B0466201}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C71302-8399-454B-AADA-CD30E2FA9F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -478,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -893,7 +893,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B30">
         <v>2023</v>

</xml_diff>

<commit_message>
actualizacion del codigo y etiquetas de los hitos
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\kk\new_website_ECOINF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4C71302-8399-454B-AADA-CD30E2FA9F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270A51B1-21D9-46AF-A28F-29AAFC1FA473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
   <si>
     <t>month</t>
   </si>
@@ -148,6 +148,139 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=txJfuPeodQw</t>
+  </si>
+  <si>
+    <t>https://ecoinfaeet.github.io/new_website/</t>
+  </si>
+  <si>
+    <t>titulo</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.7818/ECOS.1591</t>
+  </si>
+  <si>
+    <t>Cómo escribir funciones en R</t>
+  </si>
+  <si>
+    <t>Cómo crear paquetes en R</t>
+  </si>
+  <si>
+    <t>Estadística circular aplicada a la Ecología</t>
+  </si>
+  <si>
+    <t>rOpenSci: cómo acceder 
+de forma reproducible a repositorios 
+de datos públicos</t>
+  </si>
+  <si>
+    <t>Ajuste, interpretación y presentación de 
+modelos lineales: el valor p no es suficiente</t>
+  </si>
+  <si>
+    <t>Procesadores de texto Markup: 
+más allá de MS Word</t>
+  </si>
+  <si>
+    <t>Sobre el intercambio de datos de vegetación: 
+el estándar ‘Veg-X’ y el paquete de R ‘VegX’</t>
+  </si>
+  <si>
+    <t>¿Por qué usar GitHub? Diez pasos para 
+disfrutar de GitHub y no morir en el intento</t>
+  </si>
+  <si>
+    <t>Ventajas de la estadística bayesiana frente 
+a la frecuentista: ¿por qué nos resistimos a usarla?</t>
+  </si>
+  <si>
+    <t>Inferencia estadística a partir de varios 
+modelos y su utilidad en ecología</t>
+  </si>
+  <si>
+    <t>Compartiendo datos en Ecología: 
+cómo añadir más valor a los datos</t>
+  </si>
+  <si>
+    <t>Quince consejos para mejorar nuestro 
+código y flujo de trabajo con R</t>
+  </si>
+  <si>
+    <t>Cómo aplicar la cienciometría 
+a la investigación ecológica</t>
+  </si>
+  <si>
+    <t>¡Se puede entender cómo 
+funcionan Git y GitHub!</t>
+  </si>
+  <si>
+    <t>La unión hace la fuerza: 
+modelos de distribución de especies 
+integrando diferentes fuentes de datos</t>
+  </si>
+  <si>
+    <t>Camelot: Una herramienta intuitiva 
+para el manejo y procesamiento de imágenes de 
+cámaras trampa utilizando inteligencia artificial</t>
+  </si>
+  <si>
+    <t>Tidyverse: colección de paquetes 
+de R para la ciencia de datos</t>
+  </si>
+  <si>
+    <t>Búsqueda, descarga y limpieza 
+de datos desde GBIF</t>
+  </si>
+  <si>
+    <t>Estadística bayesiana</t>
+  </si>
+  <si>
+    <t>Análisis de la ciencia ciudadana 
+mediante modelos de ocupación</t>
+  </si>
+  <si>
+    <t>Generación de visores de 
+datos espaciales con R</t>
+  </si>
+  <si>
+    <t>Análisis de dinámicas poblacionales en R</t>
+  </si>
+  <si>
+    <t>Introducción a Python</t>
+  </si>
+  <si>
+    <t>Integración de datos en la estima 
+de la distribución y abundancia animal</t>
+  </si>
+  <si>
+    <t>Introducción al análisis 
+espacial de patrones de puntos</t>
+  </si>
+  <si>
+    <t>Introducción al mundo de la bioacústica</t>
+  </si>
+  <si>
+    <t>Introducción a Zotero</t>
+  </si>
+  <si>
+    <t>Introducción al uso de filogenias</t>
+  </si>
+  <si>
+    <t>Regímenes dinámicos ecológicos</t>
+  </si>
+  <si>
+    <t>labeleR: genera tus certificados y etiquetas</t>
+  </si>
+  <si>
+    <t>¿Qué información puedo obtener 
+de los datos PNOA-LiDAR?</t>
+  </si>
+  <si>
+    <t>Inferir rango de distribución a 
+partir de diversidad genética</t>
+  </si>
+  <si>
+    <t>El papel de la IA en la ecología, 
+cómo transformar imágenes en datos</t>
   </si>
 </sst>
 </file>
@@ -192,9 +325,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -476,19 +612,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="19.7265625" customWidth="1"/>
     <col min="3" max="3" width="38.36328125" customWidth="1"/>
+    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +638,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -512,8 +652,11 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>10</v>
       </c>
@@ -523,11 +666,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -540,8 +683,11 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6</v>
       </c>
@@ -551,11 +697,14 @@
       <c r="C5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E5" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>11</v>
       </c>
@@ -565,11 +714,14 @@
       <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>3</v>
       </c>
@@ -579,11 +731,14 @@
       <c r="C7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E7" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="174" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -593,11 +748,14 @@
       <c r="C8" t="s">
         <v>25</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -607,11 +765,14 @@
       <c r="C9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -621,11 +782,14 @@
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E10" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>11</v>
       </c>
@@ -635,11 +799,14 @@
       <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -649,11 +816,14 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -663,11 +833,14 @@
       <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E13" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>5</v>
       </c>
@@ -677,11 +850,14 @@
       <c r="C14" t="s">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -691,11 +867,14 @@
       <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E15" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>6</v>
       </c>
@@ -705,11 +884,14 @@
       <c r="C16" t="s">
         <v>25</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E16" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>12</v>
       </c>
@@ -719,11 +901,14 @@
       <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E17" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -733,11 +918,14 @@
       <c r="C18" t="s">
         <v>25</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E18" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6</v>
       </c>
@@ -747,11 +935,14 @@
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E19" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>8</v>
       </c>
@@ -764,8 +955,11 @@
       <c r="D20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E20" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -775,11 +969,14 @@
       <c r="C21" t="s">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E21" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -789,11 +986,14 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E22" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3</v>
       </c>
@@ -803,11 +1003,14 @@
       <c r="C23" t="s">
         <v>5</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E23" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>5</v>
       </c>
@@ -820,8 +1023,11 @@
       <c r="D24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E24" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>6</v>
       </c>
@@ -834,8 +1040,11 @@
       <c r="D25" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E25" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>7</v>
       </c>
@@ -848,8 +1057,11 @@
       <c r="D26" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E26" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>9</v>
       </c>
@@ -862,8 +1074,11 @@
       <c r="D27" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>10</v>
       </c>
@@ -876,8 +1091,11 @@
       <c r="D28" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>11</v>
       </c>
@@ -890,8 +1108,11 @@
       <c r="D29" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E29" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3</v>
       </c>
@@ -904,8 +1125,11 @@
       <c r="D30" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E30" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>5</v>
       </c>
@@ -918,8 +1142,11 @@
       <c r="D31" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E31" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>9</v>
       </c>
@@ -932,8 +1159,11 @@
       <c r="D32" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E32" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -946,8 +1176,11 @@
       <c r="D33" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E33" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>3</v>
       </c>
@@ -960,8 +1193,11 @@
       <c r="D34" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E34" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="116" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>4</v>
       </c>
@@ -974,8 +1210,11 @@
       <c r="D35" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E35" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>5</v>
       </c>
@@ -987,11 +1226,34 @@
       </c>
       <c r="D36" t="s">
         <v>40</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{B5274820-F334-49F2-9C65-BC403D5350B7}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{6EBAFA3B-B2F0-45F6-951F-4D8B1064B063}"/>
+    <hyperlink ref="D3" r:id="rId3" xr:uid="{CF71B0EE-DA39-43CB-83C1-1A7ACCD20076}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{C2C6E6B2-539C-400F-A20B-9060CA9373B6}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{E1B381D2-8052-4C8B-97B3-311E59DE5F30}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{78437E75-9C9E-48F9-A0D3-8ACA414C68AB}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{3C798AD5-B3FB-4188-84B4-470CB6ED69B8}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{D2C4D91F-6262-4A5D-BEF8-6AB603974389}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{9EDE0F5C-3B08-4BFD-B83E-932312E9976A}"/>
+    <hyperlink ref="D12" r:id="rId10" xr:uid="{4B8457A5-8676-499B-9C1D-4CB226E1C614}"/>
+    <hyperlink ref="D14" r:id="rId11" xr:uid="{8577162C-E63C-4ACC-9C95-C5B28E37C309}"/>
+    <hyperlink ref="D15" r:id="rId12" xr:uid="{398E5209-9D76-492C-BFCE-B4626DE88147}"/>
+    <hyperlink ref="D17" r:id="rId13" xr:uid="{45E7E255-BDE5-4896-A1CA-B06330880EA8}"/>
+    <hyperlink ref="D19" r:id="rId14" xr:uid="{8BE493EC-DD6E-42D1-9EF8-C3DA113C4CF7}"/>
+    <hyperlink ref="D21" r:id="rId15" xr:uid="{8DCACB60-4B90-4A39-B11A-2A2A474761F8}"/>
+    <hyperlink ref="D22" r:id="rId16" xr:uid="{E8E2B09A-039D-4925-8081-7F92AC13837B}"/>
+    <hyperlink ref="D11" r:id="rId17" xr:uid="{35204F6C-7389-41C7-8CF4-B711F7A915A7}"/>
+    <hyperlink ref="D13" r:id="rId18" xr:uid="{A930F9F4-CD0D-4330-BDFE-F6F1753610CC}"/>
+    <hyperlink ref="D16" r:id="rId19" xr:uid="{A85240B0-C8E7-45A1-A9AB-B8E15A972011}"/>
+    <hyperlink ref="D18" r:id="rId20" xr:uid="{FD95CFC5-9A2D-4FBE-87B2-2338AE65BEFB}"/>
+    <hyperlink ref="D23" r:id="rId21" xr:uid="{60288E13-EF5B-4C40-8C1D-869D1FCD4AF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
linea del tiempo y actividades
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro\Desktop\kk\new_website_ECOINF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/veronica_cruz_uah_es/Documents/Disco/Ecoinformatica/website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270A51B1-21D9-46AF-A28F-29AAFC1FA473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{270A51B1-21D9-46AF-A28F-29AAFC1FA473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EC0B638-6011-4B4E-BC4B-C6BF53312AEB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="79">
   <si>
     <t>month</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=txJfuPeodQw</t>
-  </si>
-  <si>
-    <t>https://ecoinfaeet.github.io/new_website/</t>
   </si>
   <si>
     <t>titulo</t>
@@ -281,6 +278,16 @@
   <si>
     <t>El papel de la IA en la ecología, 
 cómo transformar imágenes en datos</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=XCrrR3_MSHc</t>
+  </si>
+  <si>
+    <t>BlueCarbon R package: get stocks and sequestration 
+rates estimations directly from raw laboratory data</t>
+  </si>
+  <si>
+    <t>https://ecoinfaeet.github.io</t>
   </si>
 </sst>
 </file>
@@ -347,6 +354,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,20 +623,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7265625" customWidth="1"/>
-    <col min="3" max="3" width="38.36328125" customWidth="1"/>
-    <col min="4" max="4" width="45.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.42578125" customWidth="1"/>
+    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -639,40 +650,43 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>2024</v>
+        <v>2017</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>2017</v>
@@ -681,15 +695,15 @@
         <v>25</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2017</v>
@@ -698,32 +712,32 @@
         <v>25</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>2018</v>
@@ -732,15 +746,15 @@
         <v>25</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="174" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>2018</v>
@@ -749,32 +763,32 @@
         <v>25</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C9" t="s">
         <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>2019</v>
@@ -783,66 +797,66 @@
         <v>25</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B12">
+        <v>2019</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>5</v>
+      </c>
+      <c r="B13">
         <v>2020</v>
       </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="C13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13">
-        <v>2019</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>2020</v>
@@ -851,32 +865,32 @@
         <v>25</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C15" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B16">
         <v>2021</v>
@@ -885,49 +899,49 @@
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="210" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B17">
-        <v>2021</v>
+        <v>2023</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" ht="300" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C18" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="275.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>2024</v>
@@ -935,31 +949,28 @@
       <c r="C19" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>20</v>
+      <c r="D19" t="s">
+        <v>19</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B20">
         <v>2024</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -973,10 +984,10 @@
         <v>24</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2</v>
       </c>
@@ -990,10 +1001,10 @@
         <v>26</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1007,10 +1018,10 @@
         <v>27</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1024,10 +1035,10 @@
         <v>28</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="101.5" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1041,10 +1052,10 @@
         <v>29</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1058,10 +1069,10 @@
         <v>30</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1075,10 +1086,10 @@
         <v>31</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1092,10 +1103,10 @@
         <v>32</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1109,10 +1120,10 @@
         <v>33</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1126,10 +1137,10 @@
         <v>34</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1143,10 +1154,10 @@
         <v>35</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1160,10 +1171,10 @@
         <v>36</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1177,10 +1188,10 @@
         <v>37</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1194,10 +1205,10 @@
         <v>38</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="116" x14ac:dyDescent="0.35">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1211,10 +1222,10 @@
         <v>39</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="130.5" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1228,32 +1239,53 @@
         <v>40</v>
       </c>
       <c r="E36" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>2025</v>
+      </c>
+      <c r="C37" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="E37" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+    <sortCondition ref="C1:C36"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{B5274820-F334-49F2-9C65-BC403D5350B7}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{B5274820-F334-49F2-9C65-BC403D5350B7}"/>
     <hyperlink ref="D2" r:id="rId2" xr:uid="{6EBAFA3B-B2F0-45F6-951F-4D8B1064B063}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{CF71B0EE-DA39-43CB-83C1-1A7ACCD20076}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{C2C6E6B2-539C-400F-A20B-9060CA9373B6}"/>
-    <hyperlink ref="D7" r:id="rId5" xr:uid="{E1B381D2-8052-4C8B-97B3-311E59DE5F30}"/>
-    <hyperlink ref="D6" r:id="rId6" xr:uid="{78437E75-9C9E-48F9-A0D3-8ACA414C68AB}"/>
-    <hyperlink ref="D8" r:id="rId7" xr:uid="{3C798AD5-B3FB-4188-84B4-470CB6ED69B8}"/>
-    <hyperlink ref="D9" r:id="rId8" xr:uid="{D2C4D91F-6262-4A5D-BEF8-6AB603974389}"/>
-    <hyperlink ref="D10" r:id="rId9" xr:uid="{9EDE0F5C-3B08-4BFD-B83E-932312E9976A}"/>
-    <hyperlink ref="D12" r:id="rId10" xr:uid="{4B8457A5-8676-499B-9C1D-4CB226E1C614}"/>
-    <hyperlink ref="D14" r:id="rId11" xr:uid="{8577162C-E63C-4ACC-9C95-C5B28E37C309}"/>
-    <hyperlink ref="D15" r:id="rId12" xr:uid="{398E5209-9D76-492C-BFCE-B4626DE88147}"/>
-    <hyperlink ref="D17" r:id="rId13" xr:uid="{45E7E255-BDE5-4896-A1CA-B06330880EA8}"/>
-    <hyperlink ref="D19" r:id="rId14" xr:uid="{8BE493EC-DD6E-42D1-9EF8-C3DA113C4CF7}"/>
+    <hyperlink ref="D20" r:id="rId3" xr:uid="{CF71B0EE-DA39-43CB-83C1-1A7ACCD20076}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{C2C6E6B2-539C-400F-A20B-9060CA9373B6}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{E1B381D2-8052-4C8B-97B3-311E59DE5F30}"/>
+    <hyperlink ref="D5" r:id="rId6" xr:uid="{78437E75-9C9E-48F9-A0D3-8ACA414C68AB}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{3C798AD5-B3FB-4188-84B4-470CB6ED69B8}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{D2C4D91F-6262-4A5D-BEF8-6AB603974389}"/>
+    <hyperlink ref="D9" r:id="rId9" xr:uid="{9EDE0F5C-3B08-4BFD-B83E-932312E9976A}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{4B8457A5-8676-499B-9C1D-4CB226E1C614}"/>
+    <hyperlink ref="D13" r:id="rId11" xr:uid="{8577162C-E63C-4ACC-9C95-C5B28E37C309}"/>
+    <hyperlink ref="D14" r:id="rId12" xr:uid="{398E5209-9D76-492C-BFCE-B4626DE88147}"/>
+    <hyperlink ref="D16" r:id="rId13" xr:uid="{45E7E255-BDE5-4896-A1CA-B06330880EA8}"/>
+    <hyperlink ref="D18" r:id="rId14" xr:uid="{8BE493EC-DD6E-42D1-9EF8-C3DA113C4CF7}"/>
     <hyperlink ref="D21" r:id="rId15" xr:uid="{8DCACB60-4B90-4A39-B11A-2A2A474761F8}"/>
     <hyperlink ref="D22" r:id="rId16" xr:uid="{E8E2B09A-039D-4925-8081-7F92AC13837B}"/>
-    <hyperlink ref="D11" r:id="rId17" xr:uid="{35204F6C-7389-41C7-8CF4-B711F7A915A7}"/>
-    <hyperlink ref="D13" r:id="rId18" xr:uid="{A930F9F4-CD0D-4330-BDFE-F6F1753610CC}"/>
-    <hyperlink ref="D16" r:id="rId19" xr:uid="{A85240B0-C8E7-45A1-A9AB-B8E15A972011}"/>
-    <hyperlink ref="D18" r:id="rId20" xr:uid="{FD95CFC5-9A2D-4FBE-87B2-2338AE65BEFB}"/>
+    <hyperlink ref="D10" r:id="rId17" xr:uid="{35204F6C-7389-41C7-8CF4-B711F7A915A7}"/>
+    <hyperlink ref="D12" r:id="rId18" xr:uid="{A930F9F4-CD0D-4330-BDFE-F6F1753610CC}"/>
+    <hyperlink ref="D15" r:id="rId19" xr:uid="{A85240B0-C8E7-45A1-A9AB-B8E15A972011}"/>
+    <hyperlink ref="D17" r:id="rId20" xr:uid="{FD95CFC5-9A2D-4FBE-87B2-2338AE65BEFB}"/>
     <hyperlink ref="D23" r:id="rId21" xr:uid="{60288E13-EF5B-4C40-8C1D-869D1FCD4AF3}"/>
+    <hyperlink ref="D37" r:id="rId22" xr:uid="{EC2B4E9A-8AEC-4854-A5D0-63A4DFFFF640}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update link 1st hito
</commit_message>
<xml_diff>
--- a/input_hitos.xlsx
+++ b/input_hitos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidaddealcala-my.sharepoint.com/personal/veronica_cruz_uah_es/Documents/Disco/Ecoinformatica/website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elenaqb/Documents/PROJECTS/new_website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{270A51B1-21D9-46AF-A28F-29AAFC1FA473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EC0B638-6011-4B4E-BC4B-C6BF53312AEB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFCB1EB5-CBB4-9A48-9055-110E8FF54E0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36640" yWindow="-4780" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -287,7 +287,7 @@
 rates estimations directly from raw laboratory data</t>
   </si>
   <si>
-    <t>https://ecoinfaeet.github.io</t>
+    <t>https://doi.org/10.7818/ECOS.2016.25-1.17</t>
   </si>
 </sst>
 </file>
@@ -625,18 +625,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="45.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="38.5" customWidth="1"/>
+    <col min="4" max="4" width="45.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +653,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -667,7 +667,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>3</v>
       </c>
@@ -684,7 +684,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>6</v>
       </c>
@@ -701,7 +701,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>11</v>
       </c>
@@ -718,7 +718,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -735,7 +735,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
@@ -752,7 +752,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="192" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -769,7 +769,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -786,7 +786,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>11</v>
       </c>
@@ -803,7 +803,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -820,7 +820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -837,7 +837,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>5</v>
       </c>
@@ -854,7 +854,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -871,7 +871,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>6</v>
       </c>
@@ -888,7 +888,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -905,7 +905,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="210" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -922,7 +922,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="300" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="288" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -939,7 +939,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>8</v>
       </c>
@@ -956,7 +956,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>10</v>
       </c>
@@ -970,7 +970,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -987,7 +987,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -1021,7 +1021,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>6</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="112" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>10</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>11</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>3</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>5</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>9</v>
       </c>
@@ -1174,7 +1174,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="96" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -1191,7 +1191,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>3</v>
       </c>
@@ -1208,7 +1208,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="128" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>5</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="240" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="224" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -1260,7 +1260,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E36">
+  <sortState ref="A2:E36">
     <sortCondition ref="C1:C36"/>
   </sortState>
   <hyperlinks>

</xml_diff>